<commit_message>
Commit after Excel data updated
</commit_message>
<xml_diff>
--- a/Sample/TestData/testdata1.xlsx
+++ b/Sample/TestData/testdata1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="10515" windowHeight="4695"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="11820" windowHeight="6330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -24,9 +25,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>alagappan.n@vmokshgroup.com</t>
-  </si>
-  <si>
     <t>Power@1234</t>
   </si>
   <si>
@@ -34,6 +32,9 @@
   </si>
   <si>
     <t>Power@123</t>
+  </si>
+  <si>
+    <t>admin@mydomain.com</t>
   </si>
 </sst>
 </file>
@@ -400,36 +401,34 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4"/>
-    <hyperlink ref="B4" r:id="rId5"/>
-    <hyperlink ref="A4" r:id="rId6"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
File Upload and Tool tip capture scripts commited
</commit_message>
<xml_diff>
--- a/Sample/TestData/testdata1.xlsx
+++ b/Sample/TestData/testdata1.xlsx
@@ -19,12 +19,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>Power@1234</t>
   </si>
   <si>
@@ -35,6 +29,12 @@
   </si>
   <si>
     <t>admin@mydomain.com</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -382,7 +382,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -393,34 +393,34 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>